<commit_message>
Complete remoddeling of observations and enabling of tensorboard
</commit_message>
<xml_diff>
--- a/doc/observations/Observations_PathToObs.xlsx
+++ b/doc/observations/Observations_PathToObs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dano\Documents\ZHAW\projektarbeit-zhaw\projektarbeit-2019\projektarbeit-2019\doc\observations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BFE0C2-4AD3-4C48-AF9B-054D5EC5527F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BE34F9-A296-4075-ABB0-A3C80B40E73F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{541DCEF1-EAD6-46C4-A486-1D7B6E3EE60A}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>x</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>P1</t>
-  </si>
-  <si>
-    <t>P2</t>
   </si>
   <si>
     <t>P1 = (16,18)</t>
@@ -61,12 +58,108 @@
   <si>
     <t>P1 - pos + offset = P1'</t>
   </si>
+  <si>
+    <t>Size: 21</t>
+  </si>
+  <si>
+    <t>M[Max(pos - offset,0): Min(pos + offset,size)]</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>3,3</t>
+  </si>
+  <si>
+    <t>8,8</t>
+  </si>
+  <si>
+    <t>10,10</t>
+  </si>
+  <si>
+    <t>21,21</t>
+  </si>
+  <si>
+    <t>max(pos-offset,0)</t>
+  </si>
+  <si>
+    <t>P(0,3) -&gt; P(1,4)</t>
+  </si>
+  <si>
+    <t>POS(2,2) - OFFSET(3,3) = (-1,-1)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>POS(10,10)</t>
+  </si>
+  <si>
+    <t>OFFSET(11,11)</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>MAP</t>
+  </si>
+  <si>
+    <t>OBS</t>
+  </si>
+  <si>
+    <t>OFFSET = 10</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>MIN(POS + OFF,</t>
+  </si>
+  <si>
+    <t>MAX(POS-OFF,0)</t>
+  </si>
+  <si>
+    <t>2 bis 16</t>
+  </si>
+  <si>
+    <t>SIZE</t>
+  </si>
+  <si>
+    <t>Size Obs</t>
+  </si>
+  <si>
+    <t>Size Env</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>P1'</t>
+  </si>
+  <si>
+    <t>P1' Calc</t>
+  </si>
+  <si>
+    <t>POS - OFFSET = OFFSET ZUM ENV</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,8 +174,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,8 +206,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -116,11 +245,110 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -135,6 +363,75 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -451,121 +748,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134D699B-9D30-405A-98F5-D6C9211C8736}">
-  <dimension ref="A1:CD82"/>
+  <dimension ref="A1:CD133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AN109" sqref="AN109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="2"/>
-    <col min="2" max="82" width="3.53125" style="2" customWidth="1"/>
+    <col min="2" max="33" width="3.53125" style="2" customWidth="1"/>
+    <col min="34" max="34" width="9.46484375" style="25" customWidth="1"/>
+    <col min="35" max="35" width="10.1328125" style="25" customWidth="1"/>
+    <col min="36" max="82" width="3.53125" style="2" customWidth="1"/>
     <col min="83" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:82" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="2">
+      <c r="D1" s="2">
         <v>0</v>
       </c>
-      <c r="C1" s="2">
+      <c r="E1" s="2">
         <v>1</v>
       </c>
-      <c r="D1" s="2">
+      <c r="F1" s="2">
         <v>2</v>
       </c>
-      <c r="E1" s="2">
+      <c r="G1" s="2">
         <v>3</v>
       </c>
-      <c r="F1" s="2">
+      <c r="H1" s="2">
         <v>4</v>
       </c>
-      <c r="G1" s="2">
+      <c r="I1" s="2">
         <v>5</v>
       </c>
-      <c r="H1" s="2">
+      <c r="J1" s="2">
         <v>6</v>
       </c>
-      <c r="I1" s="2">
+      <c r="K1" s="2">
         <v>7</v>
       </c>
-      <c r="J1" s="2">
+      <c r="L1" s="2">
         <v>8</v>
       </c>
-      <c r="K1" s="2">
+      <c r="M1" s="2">
         <v>9</v>
       </c>
-      <c r="L1" s="2">
+      <c r="N1" s="2">
         <v>10</v>
       </c>
-      <c r="M1" s="2">
+      <c r="O1" s="2">
         <v>11</v>
       </c>
-      <c r="N1" s="2">
+      <c r="P1" s="2">
         <v>12</v>
       </c>
-      <c r="O1" s="2">
+      <c r="Q1" s="2">
         <v>13</v>
       </c>
-      <c r="P1" s="2">
+      <c r="R1" s="2">
         <v>14</v>
       </c>
-      <c r="Q1" s="2">
+      <c r="S1" s="2">
         <v>15</v>
       </c>
-      <c r="R1" s="2">
+      <c r="T1" s="2">
         <v>16</v>
       </c>
-      <c r="S1" s="2">
+      <c r="U1" s="2">
         <v>17</v>
       </c>
-      <c r="T1" s="2">
+      <c r="V1" s="2">
         <v>18</v>
       </c>
-      <c r="U1" s="2">
+      <c r="W1" s="2">
         <v>19</v>
       </c>
-      <c r="V1" s="2">
+      <c r="X1" s="2">
         <v>20</v>
       </c>
-      <c r="W1" s="2">
+      <c r="Y1" s="2">
         <v>21</v>
       </c>
-      <c r="X1" s="2">
+      <c r="Z1" s="2">
         <v>22</v>
       </c>
-      <c r="Y1" s="2">
+      <c r="AA1" s="2">
         <v>23</v>
       </c>
-      <c r="Z1" s="2">
+      <c r="AB1" s="2">
         <v>24</v>
       </c>
-      <c r="AA1" s="2">
+      <c r="AC1" s="2">
         <v>25</v>
       </c>
-      <c r="AB1" s="2">
+      <c r="AD1" s="2">
         <v>26</v>
       </c>
-      <c r="AC1" s="2">
+      <c r="AE1" s="2">
         <v>27</v>
       </c>
-      <c r="AD1" s="2">
+      <c r="AF1" s="2">
         <v>28</v>
       </c>
-      <c r="AE1" s="2">
+      <c r="AG1" s="2">
         <v>29</v>
       </c>
-      <c r="AF1" s="2">
+      <c r="AH1" s="25">
         <v>30</v>
       </c>
-      <c r="AG1" s="2">
-        <v>31</v>
-      </c>
-      <c r="AH1" s="2">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="2">
+      <c r="AI1" s="25">
         <v>33</v>
       </c>
       <c r="AJ1" s="2">
@@ -711,33 +1005,76 @@
       </c>
     </row>
     <row r="2" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="2">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7">
+        <v>2</v>
+      </c>
+      <c r="F2" s="7">
+        <v>3</v>
+      </c>
+      <c r="G2" s="7">
+        <v>4</v>
+      </c>
+      <c r="H2" s="7">
+        <v>5</v>
+      </c>
+      <c r="I2" s="7">
+        <v>6</v>
+      </c>
+      <c r="J2" s="7">
+        <v>7</v>
+      </c>
+      <c r="K2" s="7">
+        <v>8</v>
+      </c>
+      <c r="L2" s="7">
+        <v>9</v>
+      </c>
+      <c r="M2" s="7">
+        <v>10</v>
+      </c>
+      <c r="N2" s="7">
+        <v>11</v>
+      </c>
+      <c r="O2" s="7">
+        <v>12</v>
+      </c>
+      <c r="P2" s="7">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>14</v>
+      </c>
+      <c r="R2" s="7">
+        <v>15</v>
+      </c>
+      <c r="S2" s="7">
+        <v>16</v>
+      </c>
+      <c r="T2" s="7">
+        <v>17</v>
+      </c>
+      <c r="U2" s="7">
+        <v>18</v>
+      </c>
+      <c r="V2" s="7">
+        <v>19</v>
+      </c>
+      <c r="W2" s="7">
+        <v>20</v>
+      </c>
+      <c r="X2" s="7">
+        <v>21</v>
+      </c>
+      <c r="Y2" s="7">
+        <v>22</v>
+      </c>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
@@ -746,8 +1083,8 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
       <c r="AL2" s="1"/>
@@ -797,33 +1134,34 @@
       <c r="CD2" s="1"/>
     </row>
     <row r="3" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
@@ -832,8 +1170,8 @@
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="5"/>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
@@ -884,47 +1222,55 @@
     </row>
     <row r="4" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="4"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
+      <c r="AB4" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
-      <c r="AN4" s="1"/>
+      <c r="AN4" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
@@ -970,32 +1316,34 @@
     </row>
     <row r="5" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="B5" s="6">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="4"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
@@ -1004,13 +1352,15 @@
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="1"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
       <c r="AL5" s="1"/>
       <c r="AM5" s="1"/>
-      <c r="AN5" s="1"/>
+      <c r="AN5" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="AO5" s="1"/>
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
@@ -1056,42 +1406,48 @@
     </row>
     <row r="6" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="B6" s="6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="4"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
+      <c r="AD6" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
       <c r="AL6" s="1"/>
@@ -1142,42 +1498,44 @@
     </row>
     <row r="7" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="5"/>
-      <c r="AA7" s="5"/>
-      <c r="AB7" s="5"/>
-      <c r="AC7" s="5"/>
-      <c r="AD7" s="5"/>
-      <c r="AE7" s="5"/>
-      <c r="AF7" s="5"/>
-      <c r="AG7" s="5"/>
-      <c r="AH7" s="1"/>
-      <c r="AI7" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B7" s="6">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="5"/>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
       <c r="AL7" s="1"/>
@@ -1228,42 +1586,46 @@
     </row>
     <row r="8" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="B8" s="6">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="1"/>
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
       <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
+      <c r="AD8" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="AE8" s="5"/>
       <c r="AF8" s="5"/>
       <c r="AG8" s="5"/>
-      <c r="AH8" s="1"/>
-      <c r="AI8" s="1"/>
+      <c r="AH8" s="5"/>
+      <c r="AI8" s="5"/>
       <c r="AJ8" s="1"/>
       <c r="AK8" s="1"/>
       <c r="AL8" s="1"/>
@@ -1314,33 +1676,35 @@
     </row>
     <row r="9" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="B9" s="6">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="1"/>
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
       <c r="AC9" s="5"/>
@@ -1348,8 +1712,8 @@
       <c r="AE9" s="5"/>
       <c r="AF9" s="5"/>
       <c r="AG9" s="5"/>
-      <c r="AH9" s="1"/>
-      <c r="AI9" s="1"/>
+      <c r="AH9" s="5"/>
+      <c r="AI9" s="5"/>
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
       <c r="AL9" s="1"/>
@@ -1400,44 +1764,44 @@
     </row>
     <row r="10" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="B10" s="6">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="1"/>
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
       <c r="AC10" s="5"/>
-      <c r="AD10" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="AD10" s="5"/>
       <c r="AE10" s="5"/>
       <c r="AF10" s="5"/>
       <c r="AG10" s="5"/>
-      <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
+      <c r="AH10" s="5"/>
+      <c r="AI10" s="5"/>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
       <c r="AL10" s="1"/>
@@ -1488,46 +1852,46 @@
     </row>
     <row r="11" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="B11" s="6">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="1"/>
       <c r="AA11" s="5"/>
       <c r="AB11" s="5"/>
       <c r="AC11" s="5"/>
       <c r="AD11" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE11" s="5"/>
       <c r="AF11" s="5"/>
       <c r="AG11" s="5"/>
-      <c r="AH11" s="1"/>
-      <c r="AI11" s="1"/>
+      <c r="AH11" s="5"/>
+      <c r="AI11" s="5"/>
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1"/>
       <c r="AL11" s="1"/>
@@ -1578,42 +1942,46 @@
     </row>
     <row r="12" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="B12" s="6">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="1"/>
       <c r="AA12" s="5"/>
       <c r="AB12" s="5"/>
       <c r="AC12" s="5"/>
-      <c r="AD12" s="5"/>
+      <c r="AD12" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="AE12" s="5"/>
       <c r="AF12" s="5"/>
       <c r="AG12" s="5"/>
-      <c r="AH12" s="1"/>
-      <c r="AI12" s="1"/>
+      <c r="AH12" s="5"/>
+      <c r="AI12" s="5"/>
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
       <c r="AL12" s="1"/>
@@ -1664,44 +2032,44 @@
     </row>
     <row r="13" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="B13" s="6">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="1"/>
       <c r="AA13" s="5"/>
       <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
-      <c r="AD13" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="AD13" s="5"/>
       <c r="AE13" s="5"/>
       <c r="AF13" s="5"/>
       <c r="AG13" s="5"/>
-      <c r="AH13" s="1"/>
-      <c r="AI13" s="1"/>
+      <c r="AH13" s="5"/>
+      <c r="AI13" s="5"/>
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1"/>
       <c r="AL13" s="1"/>
@@ -1752,44 +2120,48 @@
     </row>
     <row r="14" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="B14" s="6">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="1"/>
       <c r="AA14" s="5"/>
       <c r="AB14" s="5"/>
       <c r="AC14" s="5"/>
       <c r="AD14" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AE14" s="5"/>
       <c r="AF14" s="5"/>
       <c r="AG14" s="5"/>
-      <c r="AH14" s="1"/>
-      <c r="AI14" s="1"/>
+      <c r="AH14" s="5"/>
+      <c r="AI14" s="5"/>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
       <c r="AL14" s="1"/>
@@ -1840,42 +2212,46 @@
     </row>
     <row r="15" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="B15" s="6">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="1"/>
       <c r="AA15" s="5"/>
       <c r="AB15" s="5"/>
       <c r="AC15" s="5"/>
-      <c r="AD15" s="5"/>
+      <c r="AD15" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="AE15" s="5"/>
       <c r="AF15" s="5"/>
       <c r="AG15" s="5"/>
-      <c r="AH15" s="1"/>
-      <c r="AI15" s="1"/>
+      <c r="AH15" s="5"/>
+      <c r="AI15" s="5"/>
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
       <c r="AL15" s="1"/>
@@ -1926,56 +2302,44 @@
     </row>
     <row r="16" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="3">
-        <v>1</v>
-      </c>
-      <c r="R16" s="3">
-        <v>2</v>
-      </c>
-      <c r="S16" s="3">
-        <v>3</v>
-      </c>
-      <c r="T16" s="3">
-        <v>4</v>
-      </c>
-      <c r="U16" s="3">
-        <v>5</v>
-      </c>
-      <c r="V16" s="3">
-        <v>6</v>
-      </c>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B16" s="6">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="4"/>
       <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
-      <c r="AE16" s="1"/>
-      <c r="AF16" s="1"/>
-      <c r="AG16" s="1"/>
-      <c r="AH16" s="1"/>
-      <c r="AI16" s="1"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="5"/>
+      <c r="AD16" s="5"/>
+      <c r="AE16" s="5"/>
+      <c r="AF16" s="5"/>
+      <c r="AG16" s="5"/>
+      <c r="AH16" s="5"/>
+      <c r="AI16" s="5"/>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
       <c r="AL16" s="1"/>
@@ -2026,46 +2390,44 @@
     </row>
     <row r="17" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3">
-        <v>0</v>
-      </c>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="B17" s="6">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="4"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
-      <c r="AD17" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
-      <c r="AH17" s="1"/>
-      <c r="AI17" s="1"/>
+      <c r="AH17" s="5"/>
+      <c r="AI17" s="5"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
       <c r="AL17" s="1"/>
@@ -2116,48 +2478,46 @@
     </row>
     <row r="18" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3">
-        <v>1</v>
-      </c>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="B18" s="6">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="4"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
       <c r="AD18" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
-      <c r="AH18" s="1"/>
-      <c r="AI18" s="1"/>
+      <c r="AH18" s="5"/>
+      <c r="AI18" s="5"/>
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
       <c r="AL18" s="1"/>
@@ -2208,44 +2568,46 @@
     </row>
     <row r="19" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3">
-        <v>2</v>
-      </c>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="B19" s="6">
+        <v>16</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="4"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
-      <c r="AD19" s="1"/>
+      <c r="AD19" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
       <c r="AG19" s="1"/>
-      <c r="AH19" s="1"/>
-      <c r="AI19" s="1"/>
+      <c r="AH19" s="5"/>
+      <c r="AI19" s="5"/>
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
       <c r="AL19" s="1"/>
@@ -2296,48 +2658,44 @@
     </row>
     <row r="20" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3">
-        <v>3</v>
-      </c>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B20" s="6">
+        <v>17</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="4"/>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
-      <c r="AD20" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="AD20" s="1"/>
       <c r="AE20" s="1"/>
       <c r="AF20" s="1"/>
       <c r="AG20" s="1"/>
-      <c r="AH20" s="1"/>
-      <c r="AI20" s="1"/>
+      <c r="AH20" s="5"/>
+      <c r="AI20" s="5"/>
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
       <c r="AL20" s="1"/>
@@ -2388,44 +2746,46 @@
     </row>
     <row r="21" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
-        <v>19</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3">
-        <v>4</v>
-      </c>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="B21" s="6">
+        <v>18</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="4"/>
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
-      <c r="AD21" s="1"/>
+      <c r="AD21" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
       <c r="AG21" s="1"/>
-      <c r="AH21" s="1"/>
-      <c r="AI21" s="1"/>
+      <c r="AH21" s="5"/>
+      <c r="AI21" s="5"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
       <c r="AL21" s="1"/>
@@ -2476,34 +2836,34 @@
     </row>
     <row r="22" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3">
-        <v>5</v>
-      </c>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="B22" s="6">
+        <v>19</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="4"/>
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
@@ -2512,8 +2872,8 @@
       <c r="AE22" s="1"/>
       <c r="AF22" s="1"/>
       <c r="AG22" s="1"/>
-      <c r="AH22" s="1"/>
-      <c r="AI22" s="1"/>
+      <c r="AH22" s="5"/>
+      <c r="AI22" s="5"/>
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
       <c r="AL22" s="1"/>
@@ -2564,34 +2924,34 @@
     </row>
     <row r="23" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
-        <v>21</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1">
-        <v>6</v>
-      </c>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="B23" s="6">
+        <v>20</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="4"/>
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
@@ -2600,8 +2960,8 @@
       <c r="AE23" s="1"/>
       <c r="AF23" s="1"/>
       <c r="AG23" s="1"/>
-      <c r="AH23" s="1"/>
-      <c r="AI23" s="1"/>
+      <c r="AH23" s="5"/>
+      <c r="AI23" s="5"/>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
       <c r="AL23" s="1"/>
@@ -2652,32 +3012,34 @@
     </row>
     <row r="24" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="B24" s="6">
+        <v>21</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="4"/>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
@@ -2686,8 +3048,8 @@
       <c r="AE24" s="1"/>
       <c r="AF24" s="1"/>
       <c r="AG24" s="1"/>
-      <c r="AH24" s="1"/>
-      <c r="AI24" s="1"/>
+      <c r="AH24" s="5"/>
+      <c r="AI24" s="5"/>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
       <c r="AL24" s="1"/>
@@ -2738,33 +3100,35 @@
     </row>
     <row r="25" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
-        <v>23</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="B25" s="6">
+        <v>22</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="4"/>
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
@@ -2772,8 +3136,8 @@
       <c r="AE25" s="1"/>
       <c r="AF25" s="1"/>
       <c r="AG25" s="1"/>
-      <c r="AH25" s="1"/>
-      <c r="AI25" s="1"/>
+      <c r="AH25" s="5"/>
+      <c r="AI25" s="5"/>
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
       <c r="AL25" s="1"/>
@@ -2824,10 +3188,8 @@
     </row>
     <row r="26" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
-        <v>24</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+        <v>22</v>
+      </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -2858,8 +3220,8 @@
       <c r="AE26" s="1"/>
       <c r="AF26" s="1"/>
       <c r="AG26" s="1"/>
-      <c r="AH26" s="1"/>
-      <c r="AI26" s="1"/>
+      <c r="AH26" s="5"/>
+      <c r="AI26" s="5"/>
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
       <c r="AL26" s="1"/>
@@ -2910,10 +3272,9 @@
     </row>
     <row r="27" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -2940,12 +3301,14 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
-      <c r="AD27" s="1"/>
+      <c r="AD27" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="AE27" s="1"/>
       <c r="AF27" s="1"/>
       <c r="AG27" s="1"/>
-      <c r="AH27" s="1"/>
-      <c r="AI27" s="1"/>
+      <c r="AH27" s="5"/>
+      <c r="AI27" s="5"/>
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
       <c r="AL27" s="1"/>
@@ -2996,7 +3359,7 @@
     </row>
     <row r="28" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3017,7 +3380,9 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
+      <c r="U28" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
@@ -3030,8 +3395,8 @@
       <c r="AE28" s="1"/>
       <c r="AF28" s="1"/>
       <c r="AG28" s="1"/>
-      <c r="AH28" s="1"/>
-      <c r="AI28" s="1"/>
+      <c r="AH28" s="5"/>
+      <c r="AI28" s="5"/>
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
       <c r="AL28" s="1"/>
@@ -3082,7 +3447,7 @@
     </row>
     <row r="29" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3116,8 +3481,8 @@
       <c r="AE29" s="1"/>
       <c r="AF29" s="1"/>
       <c r="AG29" s="1"/>
-      <c r="AH29" s="1"/>
-      <c r="AI29" s="1"/>
+      <c r="AH29" s="5"/>
+      <c r="AI29" s="5"/>
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
       <c r="AL29" s="1"/>
@@ -3168,7 +3533,7 @@
     </row>
     <row r="30" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3202,8 +3567,8 @@
       <c r="AE30" s="1"/>
       <c r="AF30" s="1"/>
       <c r="AG30" s="1"/>
-      <c r="AH30" s="1"/>
-      <c r="AI30" s="1"/>
+      <c r="AH30" s="5"/>
+      <c r="AI30" s="5"/>
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
       <c r="AL30" s="1"/>
@@ -3254,7 +3619,7 @@
     </row>
     <row r="31" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -3288,8 +3653,8 @@
       <c r="AE31" s="1"/>
       <c r="AF31" s="1"/>
       <c r="AG31" s="1"/>
-      <c r="AH31" s="1"/>
-      <c r="AI31" s="1"/>
+      <c r="AH31" s="5"/>
+      <c r="AI31" s="5"/>
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
       <c r="AL31" s="1"/>
@@ -3340,7 +3705,7 @@
     </row>
     <row r="32" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3374,11 +3739,9 @@
       <c r="AE32" s="1"/>
       <c r="AF32" s="1"/>
       <c r="AG32" s="1"/>
-      <c r="AH32" s="1"/>
-      <c r="AI32" s="1"/>
-      <c r="AJ32" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="AH32" s="5"/>
+      <c r="AI32" s="5"/>
+      <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
       <c r="AL32" s="1"/>
       <c r="AM32" s="1"/>
@@ -3428,7 +3791,7 @@
     </row>
     <row r="33" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -3462,9 +3825,11 @@
       <c r="AE33" s="1"/>
       <c r="AF33" s="1"/>
       <c r="AG33" s="1"/>
-      <c r="AH33" s="1"/>
-      <c r="AI33" s="1"/>
-      <c r="AJ33" s="1"/>
+      <c r="AH33" s="5"/>
+      <c r="AI33" s="5"/>
+      <c r="AJ33" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AK33" s="1"/>
       <c r="AL33" s="1"/>
       <c r="AM33" s="1"/>
@@ -3514,7 +3879,7 @@
     </row>
     <row r="34" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3548,8 +3913,8 @@
       <c r="AE34" s="1"/>
       <c r="AF34" s="1"/>
       <c r="AG34" s="1"/>
-      <c r="AH34" s="1"/>
-      <c r="AI34" s="1"/>
+      <c r="AH34" s="5"/>
+      <c r="AI34" s="5"/>
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
       <c r="AL34" s="1"/>
@@ -3600,7 +3965,7 @@
     </row>
     <row r="35" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3634,8 +3999,8 @@
       <c r="AE35" s="1"/>
       <c r="AF35" s="1"/>
       <c r="AG35" s="1"/>
-      <c r="AH35" s="1"/>
-      <c r="AI35" s="1"/>
+      <c r="AH35" s="5"/>
+      <c r="AI35" s="5"/>
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
       <c r="AL35" s="1"/>
@@ -3686,7 +4051,7 @@
     </row>
     <row r="36" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3720,8 +4085,8 @@
       <c r="AE36" s="1"/>
       <c r="AF36" s="1"/>
       <c r="AG36" s="1"/>
-      <c r="AH36" s="1"/>
-      <c r="AI36" s="1"/>
+      <c r="AH36" s="5"/>
+      <c r="AI36" s="5"/>
       <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
       <c r="AL36" s="1"/>
@@ -3772,7 +4137,7 @@
     </row>
     <row r="37" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3806,8 +4171,8 @@
       <c r="AE37" s="1"/>
       <c r="AF37" s="1"/>
       <c r="AG37" s="1"/>
-      <c r="AH37" s="1"/>
-      <c r="AI37" s="1"/>
+      <c r="AH37" s="5"/>
+      <c r="AI37" s="5"/>
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
       <c r="AL37" s="1"/>
@@ -3858,7 +4223,7 @@
     </row>
     <row r="38" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3892,8 +4257,8 @@
       <c r="AE38" s="1"/>
       <c r="AF38" s="1"/>
       <c r="AG38" s="1"/>
-      <c r="AH38" s="1"/>
-      <c r="AI38" s="1"/>
+      <c r="AH38" s="5"/>
+      <c r="AI38" s="5"/>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
       <c r="AL38" s="1"/>
@@ -3944,7 +4309,7 @@
     </row>
     <row r="39" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3978,8 +4343,8 @@
       <c r="AE39" s="1"/>
       <c r="AF39" s="1"/>
       <c r="AG39" s="1"/>
-      <c r="AH39" s="1"/>
-      <c r="AI39" s="1"/>
+      <c r="AH39" s="5"/>
+      <c r="AI39" s="5"/>
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
       <c r="AL39" s="1"/>
@@ -4030,7 +4395,7 @@
     </row>
     <row r="40" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -4064,8 +4429,8 @@
       <c r="AE40" s="1"/>
       <c r="AF40" s="1"/>
       <c r="AG40" s="1"/>
-      <c r="AH40" s="1"/>
-      <c r="AI40" s="1"/>
+      <c r="AH40" s="5"/>
+      <c r="AI40" s="5"/>
       <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
       <c r="AL40" s="1"/>
@@ -4116,7 +4481,7 @@
     </row>
     <row r="41" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -4150,8 +4515,8 @@
       <c r="AE41" s="1"/>
       <c r="AF41" s="1"/>
       <c r="AG41" s="1"/>
-      <c r="AH41" s="1"/>
-      <c r="AI41" s="1"/>
+      <c r="AH41" s="5"/>
+      <c r="AI41" s="5"/>
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1"/>
       <c r="AL41" s="1"/>
@@ -4202,7 +4567,7 @@
     </row>
     <row r="42" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -4236,8 +4601,8 @@
       <c r="AE42" s="1"/>
       <c r="AF42" s="1"/>
       <c r="AG42" s="1"/>
-      <c r="AH42" s="1"/>
-      <c r="AI42" s="1"/>
+      <c r="AH42" s="5"/>
+      <c r="AI42" s="5"/>
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
       <c r="AL42" s="1"/>
@@ -4288,7 +4653,7 @@
     </row>
     <row r="43" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -4322,8 +4687,8 @@
       <c r="AE43" s="1"/>
       <c r="AF43" s="1"/>
       <c r="AG43" s="1"/>
-      <c r="AH43" s="1"/>
-      <c r="AI43" s="1"/>
+      <c r="AH43" s="5"/>
+      <c r="AI43" s="5"/>
       <c r="AJ43" s="1"/>
       <c r="AK43" s="1"/>
       <c r="AL43" s="1"/>
@@ -4374,7 +4739,7 @@
     </row>
     <row r="44" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -4408,8 +4773,8 @@
       <c r="AE44" s="1"/>
       <c r="AF44" s="1"/>
       <c r="AG44" s="1"/>
-      <c r="AH44" s="1"/>
-      <c r="AI44" s="1"/>
+      <c r="AH44" s="5"/>
+      <c r="AI44" s="5"/>
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1"/>
       <c r="AL44" s="1"/>
@@ -4460,7 +4825,7 @@
     </row>
     <row r="45" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -4494,8 +4859,8 @@
       <c r="AE45" s="1"/>
       <c r="AF45" s="1"/>
       <c r="AG45" s="1"/>
-      <c r="AH45" s="1"/>
-      <c r="AI45" s="1"/>
+      <c r="AH45" s="5"/>
+      <c r="AI45" s="5"/>
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
       <c r="AL45" s="1"/>
@@ -4546,7 +4911,7 @@
     </row>
     <row r="46" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -4580,8 +4945,8 @@
       <c r="AE46" s="1"/>
       <c r="AF46" s="1"/>
       <c r="AG46" s="1"/>
-      <c r="AH46" s="1"/>
-      <c r="AI46" s="1"/>
+      <c r="AH46" s="5"/>
+      <c r="AI46" s="5"/>
       <c r="AJ46" s="1"/>
       <c r="AK46" s="1"/>
       <c r="AL46" s="1"/>
@@ -4632,7 +4997,7 @@
     </row>
     <row r="47" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -4666,8 +5031,8 @@
       <c r="AE47" s="1"/>
       <c r="AF47" s="1"/>
       <c r="AG47" s="1"/>
-      <c r="AH47" s="1"/>
-      <c r="AI47" s="1"/>
+      <c r="AH47" s="5"/>
+      <c r="AI47" s="5"/>
       <c r="AJ47" s="1"/>
       <c r="AK47" s="1"/>
       <c r="AL47" s="1"/>
@@ -4718,7 +5083,7 @@
     </row>
     <row r="48" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -4752,8 +5117,8 @@
       <c r="AE48" s="1"/>
       <c r="AF48" s="1"/>
       <c r="AG48" s="1"/>
-      <c r="AH48" s="1"/>
-      <c r="AI48" s="1"/>
+      <c r="AH48" s="5"/>
+      <c r="AI48" s="5"/>
       <c r="AJ48" s="1"/>
       <c r="AK48" s="1"/>
       <c r="AL48" s="1"/>
@@ -4804,7 +5169,7 @@
     </row>
     <row r="49" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -4838,8 +5203,8 @@
       <c r="AE49" s="1"/>
       <c r="AF49" s="1"/>
       <c r="AG49" s="1"/>
-      <c r="AH49" s="1"/>
-      <c r="AI49" s="1"/>
+      <c r="AH49" s="5"/>
+      <c r="AI49" s="5"/>
       <c r="AJ49" s="1"/>
       <c r="AK49" s="1"/>
       <c r="AL49" s="1"/>
@@ -4890,7 +5255,7 @@
     </row>
     <row r="50" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -4924,8 +5289,8 @@
       <c r="AE50" s="1"/>
       <c r="AF50" s="1"/>
       <c r="AG50" s="1"/>
-      <c r="AH50" s="1"/>
-      <c r="AI50" s="1"/>
+      <c r="AH50" s="5"/>
+      <c r="AI50" s="5"/>
       <c r="AJ50" s="1"/>
       <c r="AK50" s="1"/>
       <c r="AL50" s="1"/>
@@ -4976,7 +5341,7 @@
     </row>
     <row r="51" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -5010,8 +5375,8 @@
       <c r="AE51" s="1"/>
       <c r="AF51" s="1"/>
       <c r="AG51" s="1"/>
-      <c r="AH51" s="1"/>
-      <c r="AI51" s="1"/>
+      <c r="AH51" s="5"/>
+      <c r="AI51" s="5"/>
       <c r="AJ51" s="1"/>
       <c r="AK51" s="1"/>
       <c r="AL51" s="1"/>
@@ -5062,7 +5427,7 @@
     </row>
     <row r="52" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="2">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -5096,8 +5461,8 @@
       <c r="AE52" s="1"/>
       <c r="AF52" s="1"/>
       <c r="AG52" s="1"/>
-      <c r="AH52" s="1"/>
-      <c r="AI52" s="1"/>
+      <c r="AH52" s="5"/>
+      <c r="AI52" s="5"/>
       <c r="AJ52" s="1"/>
       <c r="AK52" s="1"/>
       <c r="AL52" s="1"/>
@@ -5148,7 +5513,7 @@
     </row>
     <row r="53" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="2">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -5182,8 +5547,8 @@
       <c r="AE53" s="1"/>
       <c r="AF53" s="1"/>
       <c r="AG53" s="1"/>
-      <c r="AH53" s="1"/>
-      <c r="AI53" s="1"/>
+      <c r="AH53" s="5"/>
+      <c r="AI53" s="5"/>
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
       <c r="AL53" s="1"/>
@@ -5234,7 +5599,7 @@
     </row>
     <row r="54" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="2">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -5268,8 +5633,8 @@
       <c r="AE54" s="1"/>
       <c r="AF54" s="1"/>
       <c r="AG54" s="1"/>
-      <c r="AH54" s="1"/>
-      <c r="AI54" s="1"/>
+      <c r="AH54" s="5"/>
+      <c r="AI54" s="5"/>
       <c r="AJ54" s="1"/>
       <c r="AK54" s="1"/>
       <c r="AL54" s="1"/>
@@ -5320,7 +5685,7 @@
     </row>
     <row r="55" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="2">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -5354,8 +5719,8 @@
       <c r="AE55" s="1"/>
       <c r="AF55" s="1"/>
       <c r="AG55" s="1"/>
-      <c r="AH55" s="1"/>
-      <c r="AI55" s="1"/>
+      <c r="AH55" s="5"/>
+      <c r="AI55" s="5"/>
       <c r="AJ55" s="1"/>
       <c r="AK55" s="1"/>
       <c r="AL55" s="1"/>
@@ -5406,7 +5771,7 @@
     </row>
     <row r="56" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="2">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -5440,8 +5805,8 @@
       <c r="AE56" s="1"/>
       <c r="AF56" s="1"/>
       <c r="AG56" s="1"/>
-      <c r="AH56" s="1"/>
-      <c r="AI56" s="1"/>
+      <c r="AH56" s="5"/>
+      <c r="AI56" s="5"/>
       <c r="AJ56" s="1"/>
       <c r="AK56" s="1"/>
       <c r="AL56" s="1"/>
@@ -5492,7 +5857,7 @@
     </row>
     <row r="57" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -5526,8 +5891,8 @@
       <c r="AE57" s="1"/>
       <c r="AF57" s="1"/>
       <c r="AG57" s="1"/>
-      <c r="AH57" s="1"/>
-      <c r="AI57" s="1"/>
+      <c r="AH57" s="5"/>
+      <c r="AI57" s="5"/>
       <c r="AJ57" s="1"/>
       <c r="AK57" s="1"/>
       <c r="AL57" s="1"/>
@@ -5578,7 +5943,7 @@
     </row>
     <row r="58" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="2">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -5612,8 +5977,8 @@
       <c r="AE58" s="1"/>
       <c r="AF58" s="1"/>
       <c r="AG58" s="1"/>
-      <c r="AH58" s="1"/>
-      <c r="AI58" s="1"/>
+      <c r="AH58" s="5"/>
+      <c r="AI58" s="5"/>
       <c r="AJ58" s="1"/>
       <c r="AK58" s="1"/>
       <c r="AL58" s="1"/>
@@ -5664,7 +6029,7 @@
     </row>
     <row r="59" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="2">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -5698,8 +6063,8 @@
       <c r="AE59" s="1"/>
       <c r="AF59" s="1"/>
       <c r="AG59" s="1"/>
-      <c r="AH59" s="1"/>
-      <c r="AI59" s="1"/>
+      <c r="AH59" s="5"/>
+      <c r="AI59" s="5"/>
       <c r="AJ59" s="1"/>
       <c r="AK59" s="1"/>
       <c r="AL59" s="1"/>
@@ -5750,7 +6115,7 @@
     </row>
     <row r="60" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="2">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -5784,8 +6149,8 @@
       <c r="AE60" s="1"/>
       <c r="AF60" s="1"/>
       <c r="AG60" s="1"/>
-      <c r="AH60" s="1"/>
-      <c r="AI60" s="1"/>
+      <c r="AH60" s="5"/>
+      <c r="AI60" s="5"/>
       <c r="AJ60" s="1"/>
       <c r="AK60" s="1"/>
       <c r="AL60" s="1"/>
@@ -5836,7 +6201,7 @@
     </row>
     <row r="61" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="2">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -5870,8 +6235,8 @@
       <c r="AE61" s="1"/>
       <c r="AF61" s="1"/>
       <c r="AG61" s="1"/>
-      <c r="AH61" s="1"/>
-      <c r="AI61" s="1"/>
+      <c r="AH61" s="5"/>
+      <c r="AI61" s="5"/>
       <c r="AJ61" s="1"/>
       <c r="AK61" s="1"/>
       <c r="AL61" s="1"/>
@@ -5922,7 +6287,7 @@
     </row>
     <row r="62" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="2">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -5956,8 +6321,8 @@
       <c r="AE62" s="1"/>
       <c r="AF62" s="1"/>
       <c r="AG62" s="1"/>
-      <c r="AH62" s="1"/>
-      <c r="AI62" s="1"/>
+      <c r="AH62" s="5"/>
+      <c r="AI62" s="5"/>
       <c r="AJ62" s="1"/>
       <c r="AK62" s="1"/>
       <c r="AL62" s="1"/>
@@ -6008,7 +6373,7 @@
     </row>
     <row r="63" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="2">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -6042,8 +6407,8 @@
       <c r="AE63" s="1"/>
       <c r="AF63" s="1"/>
       <c r="AG63" s="1"/>
-      <c r="AH63" s="1"/>
-      <c r="AI63" s="1"/>
+      <c r="AH63" s="5"/>
+      <c r="AI63" s="5"/>
       <c r="AJ63" s="1"/>
       <c r="AK63" s="1"/>
       <c r="AL63" s="1"/>
@@ -6094,7 +6459,7 @@
     </row>
     <row r="64" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="2">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -6128,8 +6493,8 @@
       <c r="AE64" s="1"/>
       <c r="AF64" s="1"/>
       <c r="AG64" s="1"/>
-      <c r="AH64" s="1"/>
-      <c r="AI64" s="1"/>
+      <c r="AH64" s="5"/>
+      <c r="AI64" s="5"/>
       <c r="AJ64" s="1"/>
       <c r="AK64" s="1"/>
       <c r="AL64" s="1"/>
@@ -6180,7 +6545,7 @@
     </row>
     <row r="65" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="2">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -6214,8 +6579,8 @@
       <c r="AE65" s="1"/>
       <c r="AF65" s="1"/>
       <c r="AG65" s="1"/>
-      <c r="AH65" s="1"/>
-      <c r="AI65" s="1"/>
+      <c r="AH65" s="5"/>
+      <c r="AI65" s="5"/>
       <c r="AJ65" s="1"/>
       <c r="AK65" s="1"/>
       <c r="AL65" s="1"/>
@@ -6266,7 +6631,7 @@
     </row>
     <row r="66" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="2">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -6300,8 +6665,8 @@
       <c r="AE66" s="1"/>
       <c r="AF66" s="1"/>
       <c r="AG66" s="1"/>
-      <c r="AH66" s="1"/>
-      <c r="AI66" s="1"/>
+      <c r="AH66" s="5"/>
+      <c r="AI66" s="5"/>
       <c r="AJ66" s="1"/>
       <c r="AK66" s="1"/>
       <c r="AL66" s="1"/>
@@ -6352,7 +6717,7 @@
     </row>
     <row r="67" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="2">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -6386,8 +6751,8 @@
       <c r="AE67" s="1"/>
       <c r="AF67" s="1"/>
       <c r="AG67" s="1"/>
-      <c r="AH67" s="1"/>
-      <c r="AI67" s="1"/>
+      <c r="AH67" s="5"/>
+      <c r="AI67" s="5"/>
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
       <c r="AL67" s="1"/>
@@ -6438,7 +6803,7 @@
     </row>
     <row r="68" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="2">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -6472,8 +6837,8 @@
       <c r="AE68" s="1"/>
       <c r="AF68" s="1"/>
       <c r="AG68" s="1"/>
-      <c r="AH68" s="1"/>
-      <c r="AI68" s="1"/>
+      <c r="AH68" s="5"/>
+      <c r="AI68" s="5"/>
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
       <c r="AL68" s="1"/>
@@ -6524,7 +6889,7 @@
     </row>
     <row r="69" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="2">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -6558,8 +6923,8 @@
       <c r="AE69" s="1"/>
       <c r="AF69" s="1"/>
       <c r="AG69" s="1"/>
-      <c r="AH69" s="1"/>
-      <c r="AI69" s="1"/>
+      <c r="AH69" s="5"/>
+      <c r="AI69" s="5"/>
       <c r="AJ69" s="1"/>
       <c r="AK69" s="1"/>
       <c r="AL69" s="1"/>
@@ -6610,7 +6975,7 @@
     </row>
     <row r="70" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -6644,8 +7009,8 @@
       <c r="AE70" s="1"/>
       <c r="AF70" s="1"/>
       <c r="AG70" s="1"/>
-      <c r="AH70" s="1"/>
-      <c r="AI70" s="1"/>
+      <c r="AH70" s="5"/>
+      <c r="AI70" s="5"/>
       <c r="AJ70" s="1"/>
       <c r="AK70" s="1"/>
       <c r="AL70" s="1"/>
@@ -6696,7 +7061,7 @@
     </row>
     <row r="71" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="2">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -6730,8 +7095,8 @@
       <c r="AE71" s="1"/>
       <c r="AF71" s="1"/>
       <c r="AG71" s="1"/>
-      <c r="AH71" s="1"/>
-      <c r="AI71" s="1"/>
+      <c r="AH71" s="5"/>
+      <c r="AI71" s="5"/>
       <c r="AJ71" s="1"/>
       <c r="AK71" s="1"/>
       <c r="AL71" s="1"/>
@@ -6782,7 +7147,7 @@
     </row>
     <row r="72" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="2">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -6816,8 +7181,8 @@
       <c r="AE72" s="1"/>
       <c r="AF72" s="1"/>
       <c r="AG72" s="1"/>
-      <c r="AH72" s="1"/>
-      <c r="AI72" s="1"/>
+      <c r="AH72" s="5"/>
+      <c r="AI72" s="5"/>
       <c r="AJ72" s="1"/>
       <c r="AK72" s="1"/>
       <c r="AL72" s="1"/>
@@ -6868,7 +7233,7 @@
     </row>
     <row r="73" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -6902,8 +7267,8 @@
       <c r="AE73" s="1"/>
       <c r="AF73" s="1"/>
       <c r="AG73" s="1"/>
-      <c r="AH73" s="1"/>
-      <c r="AI73" s="1"/>
+      <c r="AH73" s="5"/>
+      <c r="AI73" s="5"/>
       <c r="AJ73" s="1"/>
       <c r="AK73" s="1"/>
       <c r="AL73" s="1"/>
@@ -6954,7 +7319,7 @@
     </row>
     <row r="74" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="2">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -6988,8 +7353,8 @@
       <c r="AE74" s="1"/>
       <c r="AF74" s="1"/>
       <c r="AG74" s="1"/>
-      <c r="AH74" s="1"/>
-      <c r="AI74" s="1"/>
+      <c r="AH74" s="5"/>
+      <c r="AI74" s="5"/>
       <c r="AJ74" s="1"/>
       <c r="AK74" s="1"/>
       <c r="AL74" s="1"/>
@@ -7040,7 +7405,7 @@
     </row>
     <row r="75" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -7074,8 +7439,8 @@
       <c r="AE75" s="1"/>
       <c r="AF75" s="1"/>
       <c r="AG75" s="1"/>
-      <c r="AH75" s="1"/>
-      <c r="AI75" s="1"/>
+      <c r="AH75" s="5"/>
+      <c r="AI75" s="5"/>
       <c r="AJ75" s="1"/>
       <c r="AK75" s="1"/>
       <c r="AL75" s="1"/>
@@ -7126,7 +7491,7 @@
     </row>
     <row r="76" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -7160,8 +7525,8 @@
       <c r="AE76" s="1"/>
       <c r="AF76" s="1"/>
       <c r="AG76" s="1"/>
-      <c r="AH76" s="1"/>
-      <c r="AI76" s="1"/>
+      <c r="AH76" s="5"/>
+      <c r="AI76" s="5"/>
       <c r="AJ76" s="1"/>
       <c r="AK76" s="1"/>
       <c r="AL76" s="1"/>
@@ -7212,7 +7577,7 @@
     </row>
     <row r="77" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="2">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -7226,8 +7591,12 @@
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
-      <c r="N77" s="1"/>
-      <c r="O77" s="1"/>
+      <c r="N77" s="1">
+        <v>0</v>
+      </c>
+      <c r="O77" s="1">
+        <v>1</v>
+      </c>
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
@@ -7246,8 +7615,8 @@
       <c r="AE77" s="1"/>
       <c r="AF77" s="1"/>
       <c r="AG77" s="1"/>
-      <c r="AH77" s="1"/>
-      <c r="AI77" s="1"/>
+      <c r="AH77" s="5"/>
+      <c r="AI77" s="5"/>
       <c r="AJ77" s="1"/>
       <c r="AK77" s="1"/>
       <c r="AL77" s="1"/>
@@ -7298,7 +7667,7 @@
     </row>
     <row r="78" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="2">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -7332,8 +7701,8 @@
       <c r="AE78" s="1"/>
       <c r="AF78" s="1"/>
       <c r="AG78" s="1"/>
-      <c r="AH78" s="1"/>
-      <c r="AI78" s="1"/>
+      <c r="AH78" s="5"/>
+      <c r="AI78" s="5"/>
       <c r="AJ78" s="1"/>
       <c r="AK78" s="1"/>
       <c r="AL78" s="1"/>
@@ -7384,7 +7753,7 @@
     </row>
     <row r="79" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -7418,8 +7787,8 @@
       <c r="AE79" s="1"/>
       <c r="AF79" s="1"/>
       <c r="AG79" s="1"/>
-      <c r="AH79" s="1"/>
-      <c r="AI79" s="1"/>
+      <c r="AH79" s="5"/>
+      <c r="AI79" s="5"/>
       <c r="AJ79" s="1"/>
       <c r="AK79" s="1"/>
       <c r="AL79" s="1"/>
@@ -7470,7 +7839,7 @@
     </row>
     <row r="80" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -7481,22 +7850,52 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
+      <c r="K80" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="L80" s="1"/>
-      <c r="M80" s="1"/>
-      <c r="N80" s="1"/>
-      <c r="O80" s="1"/>
-      <c r="P80" s="1"/>
-      <c r="Q80" s="1"/>
-      <c r="R80" s="1"/>
-      <c r="S80" s="1"/>
-      <c r="T80" s="1"/>
-      <c r="U80" s="1"/>
-      <c r="V80" s="1"/>
-      <c r="W80" s="1"/>
-      <c r="X80" s="1"/>
-      <c r="Y80" s="1"/>
-      <c r="Z80" s="1"/>
+      <c r="M80" s="15">
+        <v>0</v>
+      </c>
+      <c r="N80" s="16">
+        <v>1</v>
+      </c>
+      <c r="O80" s="16">
+        <v>2</v>
+      </c>
+      <c r="P80" s="16">
+        <v>3</v>
+      </c>
+      <c r="Q80" s="16">
+        <v>4</v>
+      </c>
+      <c r="R80" s="16">
+        <v>5</v>
+      </c>
+      <c r="S80" s="16">
+        <v>6</v>
+      </c>
+      <c r="T80" s="16">
+        <v>7</v>
+      </c>
+      <c r="U80" s="16">
+        <v>8</v>
+      </c>
+      <c r="V80" s="16">
+        <v>9</v>
+      </c>
+      <c r="W80" s="16">
+        <v>10</v>
+      </c>
+      <c r="X80" s="16">
+        <v>11</v>
+      </c>
+      <c r="Y80" s="16">
+        <v>12</v>
+      </c>
+      <c r="Z80" s="17">
+        <v>13</v>
+      </c>
       <c r="AA80" s="1"/>
       <c r="AB80" s="1"/>
       <c r="AC80" s="1"/>
@@ -7504,8 +7903,8 @@
       <c r="AE80" s="1"/>
       <c r="AF80" s="1"/>
       <c r="AG80" s="1"/>
-      <c r="AH80" s="1"/>
-      <c r="AI80" s="1"/>
+      <c r="AH80" s="5"/>
+      <c r="AI80" s="5"/>
       <c r="AJ80" s="1"/>
       <c r="AK80" s="1"/>
       <c r="AL80" s="1"/>
@@ -7556,7 +7955,7 @@
     </row>
     <row r="81" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -7571,18 +7970,18 @@
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
-      <c r="O81" s="1"/>
-      <c r="P81" s="1"/>
-      <c r="Q81" s="1"/>
-      <c r="R81" s="1"/>
-      <c r="S81" s="1"/>
-      <c r="T81" s="1"/>
-      <c r="U81" s="1"/>
-      <c r="V81" s="1"/>
-      <c r="W81" s="1"/>
-      <c r="X81" s="1"/>
-      <c r="Y81" s="1"/>
-      <c r="Z81" s="1"/>
+      <c r="O81" s="3"/>
+      <c r="P81" s="3"/>
+      <c r="Q81" s="3"/>
+      <c r="R81" s="3"/>
+      <c r="S81" s="3"/>
+      <c r="T81" s="3"/>
+      <c r="U81" s="3"/>
+      <c r="V81" s="3"/>
+      <c r="W81" s="3"/>
+      <c r="X81" s="3"/>
+      <c r="Y81" s="3"/>
+      <c r="Z81" s="3"/>
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
       <c r="AC81" s="1"/>
@@ -7590,8 +7989,8 @@
       <c r="AE81" s="1"/>
       <c r="AF81" s="1"/>
       <c r="AG81" s="1"/>
-      <c r="AH81" s="1"/>
-      <c r="AI81" s="1"/>
+      <c r="AH81" s="5"/>
+      <c r="AI81" s="5"/>
       <c r="AJ81" s="1"/>
       <c r="AK81" s="1"/>
       <c r="AL81" s="1"/>
@@ -7642,7 +8041,7 @@
     </row>
     <row r="82" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -7667,7 +8066,9 @@
       <c r="V82" s="1"/>
       <c r="W82" s="1"/>
       <c r="X82" s="1"/>
-      <c r="Y82" s="1"/>
+      <c r="Y82" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="Z82" s="1"/>
       <c r="AA82" s="1"/>
       <c r="AB82" s="1"/>
@@ -7676,8 +8077,8 @@
       <c r="AE82" s="1"/>
       <c r="AF82" s="1"/>
       <c r="AG82" s="1"/>
-      <c r="AH82" s="1"/>
-      <c r="AI82" s="1"/>
+      <c r="AH82" s="5"/>
+      <c r="AI82" s="5"/>
       <c r="AJ82" s="1"/>
       <c r="AK82" s="1"/>
       <c r="AL82" s="1"/>
@@ -7726,7 +8127,1058 @@
       <c r="CC82" s="1"/>
       <c r="CD82" s="1"/>
     </row>
+    <row r="83" spans="1:82" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A83" s="2">
+        <v>80</v>
+      </c>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+      <c r="N83" s="1"/>
+      <c r="O83" s="10">
+        <v>0</v>
+      </c>
+      <c r="P83" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q83" s="11">
+        <v>2</v>
+      </c>
+      <c r="R83" s="11">
+        <v>3</v>
+      </c>
+      <c r="S83" s="11">
+        <v>4</v>
+      </c>
+      <c r="T83" s="11">
+        <v>5</v>
+      </c>
+      <c r="U83" s="11">
+        <v>6</v>
+      </c>
+      <c r="V83" s="11">
+        <v>7</v>
+      </c>
+      <c r="W83" s="11">
+        <v>8</v>
+      </c>
+      <c r="X83" s="11">
+        <v>9</v>
+      </c>
+      <c r="Y83" s="11">
+        <v>10</v>
+      </c>
+      <c r="Z83" s="11">
+        <v>11</v>
+      </c>
+      <c r="AA83" s="11"/>
+      <c r="AB83" s="11"/>
+      <c r="AC83" s="11"/>
+      <c r="AD83" s="11"/>
+      <c r="AE83" s="11"/>
+      <c r="AF83" s="11"/>
+      <c r="AG83" s="11"/>
+      <c r="AH83" s="26"/>
+      <c r="AI83" s="26"/>
+      <c r="AJ83" s="12"/>
+      <c r="AK83" s="1"/>
+      <c r="AL83" s="1"/>
+      <c r="AM83" s="1"/>
+      <c r="AN83" s="1"/>
+      <c r="AO83" s="1"/>
+      <c r="AP83" s="1"/>
+      <c r="AQ83" s="1"/>
+      <c r="AR83" s="1"/>
+      <c r="AS83" s="1"/>
+      <c r="AT83" s="1"/>
+      <c r="AU83" s="1"/>
+      <c r="AV83" s="1"/>
+      <c r="AW83" s="1"/>
+      <c r="AX83" s="1"/>
+      <c r="AY83" s="1"/>
+      <c r="AZ83" s="1"/>
+      <c r="BA83" s="1"/>
+      <c r="BB83" s="1"/>
+      <c r="BC83" s="1"/>
+      <c r="BD83" s="1"/>
+      <c r="BE83" s="1"/>
+      <c r="BF83" s="1"/>
+      <c r="BG83" s="1"/>
+      <c r="BH83" s="1"/>
+      <c r="BI83" s="1"/>
+      <c r="BJ83" s="1"/>
+      <c r="BK83" s="1"/>
+      <c r="BL83" s="1"/>
+      <c r="BM83" s="1"/>
+      <c r="BN83" s="1"/>
+      <c r="BO83" s="1"/>
+      <c r="BP83" s="1"/>
+      <c r="BQ83" s="1"/>
+      <c r="BR83" s="1"/>
+      <c r="BS83" s="1"/>
+      <c r="BT83" s="1"/>
+      <c r="BU83" s="1"/>
+      <c r="BV83" s="1"/>
+      <c r="BW83" s="1"/>
+      <c r="BX83" s="1"/>
+      <c r="BY83" s="1"/>
+      <c r="BZ83" s="1"/>
+      <c r="CA83" s="1"/>
+      <c r="CB83" s="1"/>
+      <c r="CC83" s="1"/>
+      <c r="CD83" s="1"/>
+    </row>
+    <row r="84" spans="1:82" x14ac:dyDescent="0.45">
+      <c r="O84" s="13">
+        <v>0</v>
+      </c>
+      <c r="P84" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q84" s="8">
+        <v>2</v>
+      </c>
+      <c r="R84" s="8">
+        <v>3</v>
+      </c>
+      <c r="S84" s="8">
+        <v>4</v>
+      </c>
+      <c r="T84" s="8">
+        <v>5</v>
+      </c>
+      <c r="U84" s="8">
+        <v>6</v>
+      </c>
+      <c r="V84" s="8">
+        <v>7</v>
+      </c>
+      <c r="W84" s="8">
+        <v>8</v>
+      </c>
+      <c r="X84" s="8">
+        <v>9</v>
+      </c>
+      <c r="Y84" s="8">
+        <v>10</v>
+      </c>
+      <c r="Z84" s="8">
+        <v>11</v>
+      </c>
+      <c r="AA84" s="8">
+        <v>12</v>
+      </c>
+      <c r="AB84" s="8">
+        <v>13</v>
+      </c>
+      <c r="AC84" s="8">
+        <v>14</v>
+      </c>
+      <c r="AD84" s="8">
+        <v>15</v>
+      </c>
+      <c r="AE84" s="8">
+        <v>16</v>
+      </c>
+      <c r="AF84" s="8">
+        <v>17</v>
+      </c>
+      <c r="AG84" s="8">
+        <v>18</v>
+      </c>
+      <c r="AH84" s="27">
+        <v>19</v>
+      </c>
+      <c r="AI84" s="27">
+        <v>20</v>
+      </c>
+      <c r="AJ84" s="14">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="85" spans="1:82" x14ac:dyDescent="0.45">
+      <c r="L85" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:82" x14ac:dyDescent="0.45">
+      <c r="O87" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="100" spans="12:67" x14ac:dyDescent="0.45">
+      <c r="M100" s="2">
+        <v>0</v>
+      </c>
+      <c r="N100" s="2">
+        <v>1</v>
+      </c>
+      <c r="O100" s="2">
+        <v>2</v>
+      </c>
+      <c r="P100" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="12:67" x14ac:dyDescent="0.45">
+      <c r="L101" s="2">
+        <v>0</v>
+      </c>
+      <c r="M101" s="18"/>
+      <c r="N101" s="18"/>
+      <c r="O101" s="18"/>
+      <c r="P101" s="18"/>
+      <c r="AU101" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV101" s="2">
+        <v>1</v>
+      </c>
+      <c r="AW101" s="2">
+        <v>2</v>
+      </c>
+      <c r="AX101" s="2">
+        <v>3</v>
+      </c>
+      <c r="AY101" s="2">
+        <v>4</v>
+      </c>
+      <c r="AZ101" s="2">
+        <v>5</v>
+      </c>
+      <c r="BA101" s="2">
+        <v>6</v>
+      </c>
+      <c r="BB101" s="2">
+        <v>7</v>
+      </c>
+      <c r="BC101" s="2">
+        <v>8</v>
+      </c>
+      <c r="BD101" s="2">
+        <v>9</v>
+      </c>
+      <c r="BE101" s="2">
+        <v>10</v>
+      </c>
+      <c r="BF101" s="2">
+        <v>11</v>
+      </c>
+      <c r="BG101" s="2">
+        <v>12</v>
+      </c>
+      <c r="BH101" s="2">
+        <v>13</v>
+      </c>
+      <c r="BI101" s="2">
+        <v>14</v>
+      </c>
+      <c r="BJ101" s="2">
+        <v>15</v>
+      </c>
+      <c r="BK101" s="2">
+        <v>16</v>
+      </c>
+      <c r="BL101" s="2">
+        <v>17</v>
+      </c>
+      <c r="BM101" s="2">
+        <v>18</v>
+      </c>
+      <c r="BN101" s="2">
+        <v>19</v>
+      </c>
+      <c r="BO101" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" spans="12:67" x14ac:dyDescent="0.45">
+      <c r="L102" s="2">
+        <v>1</v>
+      </c>
+      <c r="M102" s="18"/>
+      <c r="N102" s="18"/>
+      <c r="O102" s="18">
+        <v>0</v>
+      </c>
+      <c r="P102" s="18">
+        <v>1</v>
+      </c>
+      <c r="Q102" s="2">
+        <v>2</v>
+      </c>
+      <c r="AT102" s="2">
+        <v>0</v>
+      </c>
+      <c r="AU102" s="23"/>
+      <c r="AV102" s="23"/>
+      <c r="AW102" s="23"/>
+      <c r="AX102" s="23"/>
+      <c r="AY102" s="23"/>
+      <c r="AZ102" s="23"/>
+      <c r="BA102" s="23"/>
+      <c r="BB102" s="23"/>
+      <c r="BC102" s="23"/>
+      <c r="BD102" s="23"/>
+      <c r="BE102" s="23"/>
+      <c r="BF102" s="23"/>
+      <c r="BG102" s="23"/>
+      <c r="BH102" s="23"/>
+      <c r="BI102" s="23"/>
+      <c r="BJ102" s="23"/>
+      <c r="BK102" s="23"/>
+      <c r="BL102" s="23"/>
+      <c r="BM102" s="23"/>
+      <c r="BN102" s="23"/>
+      <c r="BO102" s="23"/>
+    </row>
+    <row r="103" spans="12:67" x14ac:dyDescent="0.45">
+      <c r="L103" s="2">
+        <v>2</v>
+      </c>
+      <c r="M103" s="18"/>
+      <c r="N103" s="18">
+        <v>0</v>
+      </c>
+      <c r="O103" s="21"/>
+      <c r="P103" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q103" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="AT103" s="2">
+        <v>1</v>
+      </c>
+      <c r="AU103" s="23"/>
+      <c r="AW103" s="2">
+        <v>0</v>
+      </c>
+      <c r="AX103" s="2">
+        <v>1</v>
+      </c>
+      <c r="AY103" s="2">
+        <v>2</v>
+      </c>
+      <c r="AZ103" s="2">
+        <v>3</v>
+      </c>
+      <c r="BA103" s="2">
+        <v>4</v>
+      </c>
+      <c r="BB103" s="2">
+        <v>5</v>
+      </c>
+      <c r="BC103" s="2">
+        <v>6</v>
+      </c>
+      <c r="BD103" s="2">
+        <v>7</v>
+      </c>
+      <c r="BE103" s="2">
+        <v>8</v>
+      </c>
+      <c r="BF103" s="2">
+        <v>9</v>
+      </c>
+      <c r="BG103" s="2">
+        <v>10</v>
+      </c>
+      <c r="BH103" s="2">
+        <v>11</v>
+      </c>
+      <c r="BI103" s="2">
+        <v>12</v>
+      </c>
+      <c r="BJ103" s="2">
+        <v>13</v>
+      </c>
+      <c r="BK103" s="23"/>
+      <c r="BL103" s="23"/>
+      <c r="BM103" s="23"/>
+      <c r="BN103" s="23"/>
+      <c r="BO103" s="23"/>
+    </row>
+    <row r="104" spans="12:67" x14ac:dyDescent="0.45">
+      <c r="L104" s="2">
+        <v>3</v>
+      </c>
+      <c r="M104" s="18"/>
+      <c r="N104" s="18">
+        <v>1</v>
+      </c>
+      <c r="O104" s="21"/>
+      <c r="P104" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q104" s="19"/>
+      <c r="AT104" s="2">
+        <v>2</v>
+      </c>
+      <c r="AU104" s="23"/>
+      <c r="AV104" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW104" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="AX104" s="24"/>
+      <c r="AY104" s="24"/>
+      <c r="AZ104" s="24"/>
+      <c r="BA104" s="24"/>
+      <c r="BB104" s="24"/>
+      <c r="BC104" s="24"/>
+      <c r="BD104" s="24"/>
+      <c r="BE104" s="24"/>
+      <c r="BF104" s="24"/>
+      <c r="BG104" s="24"/>
+      <c r="BH104" s="24"/>
+      <c r="BI104" s="24"/>
+      <c r="BJ104" s="24"/>
+      <c r="BK104" s="23"/>
+      <c r="BL104" s="23"/>
+      <c r="BM104" s="23"/>
+      <c r="BN104" s="23"/>
+      <c r="BO104" s="23"/>
+    </row>
+    <row r="105" spans="12:67" x14ac:dyDescent="0.45">
+      <c r="N105" s="2">
+        <v>2</v>
+      </c>
+      <c r="O105" s="19"/>
+      <c r="P105" s="19"/>
+      <c r="Q105" s="19"/>
+      <c r="AG105" s="2">
+        <v>14</v>
+      </c>
+      <c r="AH105" s="25">
+        <v>8</v>
+      </c>
+      <c r="AI105" s="25">
+        <v>10</v>
+      </c>
+      <c r="AJ105" s="2">
+        <v>21</v>
+      </c>
+      <c r="AT105" s="2">
+        <v>3</v>
+      </c>
+      <c r="AU105" s="23"/>
+      <c r="AV105" s="2">
+        <v>1</v>
+      </c>
+      <c r="AW105" s="24"/>
+      <c r="AX105" s="24"/>
+      <c r="AY105" s="24"/>
+      <c r="AZ105" s="24"/>
+      <c r="BA105" s="24"/>
+      <c r="BB105" s="24"/>
+      <c r="BC105" s="24"/>
+      <c r="BD105" s="24"/>
+      <c r="BE105" s="24"/>
+      <c r="BF105" s="24"/>
+      <c r="BG105" s="24"/>
+      <c r="BH105" s="24"/>
+      <c r="BI105" s="24"/>
+      <c r="BJ105" s="24"/>
+      <c r="BK105" s="23"/>
+      <c r="BL105" s="23"/>
+      <c r="BM105" s="23"/>
+      <c r="BN105" s="23"/>
+      <c r="BO105" s="23"/>
+    </row>
+    <row r="106" spans="12:67" x14ac:dyDescent="0.45">
+      <c r="AT106" s="2">
+        <v>4</v>
+      </c>
+      <c r="AU106" s="23"/>
+      <c r="AV106" s="2">
+        <v>2</v>
+      </c>
+      <c r="AW106" s="24"/>
+      <c r="AX106" s="24"/>
+      <c r="AY106" s="24"/>
+      <c r="AZ106" s="24"/>
+      <c r="BA106" s="24"/>
+      <c r="BB106" s="24"/>
+      <c r="BC106" s="24"/>
+      <c r="BD106" s="24"/>
+      <c r="BE106" s="24"/>
+      <c r="BF106" s="24"/>
+      <c r="BG106" s="24"/>
+      <c r="BH106" s="24"/>
+      <c r="BI106" s="24"/>
+      <c r="BJ106" s="24"/>
+      <c r="BK106" s="23"/>
+      <c r="BL106" s="23"/>
+      <c r="BM106" s="23"/>
+      <c r="BN106" s="23"/>
+      <c r="BO106" s="23"/>
+    </row>
+    <row r="107" spans="12:67" x14ac:dyDescent="0.45">
+      <c r="AT107" s="2">
+        <v>5</v>
+      </c>
+      <c r="AU107" s="23"/>
+      <c r="AV107" s="2">
+        <v>3</v>
+      </c>
+      <c r="AW107" s="24"/>
+      <c r="AX107" s="24"/>
+      <c r="AY107" s="24"/>
+      <c r="AZ107" s="24"/>
+      <c r="BA107" s="24"/>
+      <c r="BB107" s="24"/>
+      <c r="BC107" s="24"/>
+      <c r="BD107" s="24"/>
+      <c r="BE107" s="24"/>
+      <c r="BF107" s="24"/>
+      <c r="BG107" s="24"/>
+      <c r="BH107" s="24"/>
+      <c r="BI107" s="24"/>
+      <c r="BJ107" s="24"/>
+      <c r="BK107" s="23"/>
+      <c r="BL107" s="23"/>
+      <c r="BM107" s="23"/>
+      <c r="BN107" s="23"/>
+      <c r="BO107" s="23"/>
+    </row>
+    <row r="108" spans="12:67" x14ac:dyDescent="0.45">
+      <c r="AT108" s="2">
+        <v>6</v>
+      </c>
+      <c r="AU108" s="23"/>
+      <c r="AV108" s="2">
+        <v>4</v>
+      </c>
+      <c r="AW108" s="24"/>
+      <c r="AX108" s="24"/>
+      <c r="AY108" s="24"/>
+      <c r="AZ108" s="24"/>
+      <c r="BA108" s="24"/>
+      <c r="BB108" s="24"/>
+      <c r="BC108" s="24"/>
+      <c r="BD108" s="24"/>
+      <c r="BE108" s="24"/>
+      <c r="BF108" s="24"/>
+      <c r="BG108" s="24"/>
+      <c r="BH108" s="24"/>
+      <c r="BI108" s="24"/>
+      <c r="BJ108" s="24"/>
+      <c r="BK108" s="23"/>
+      <c r="BL108" s="23"/>
+      <c r="BM108" s="23"/>
+      <c r="BN108" s="23"/>
+      <c r="BO108" s="23"/>
+    </row>
+    <row r="109" spans="12:67" x14ac:dyDescent="0.45">
+      <c r="M109" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O109" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S109" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AT109" s="2">
+        <v>7</v>
+      </c>
+      <c r="AU109" s="23"/>
+      <c r="AV109" s="2">
+        <v>5</v>
+      </c>
+      <c r="AW109" s="24"/>
+      <c r="AX109" s="24"/>
+      <c r="AY109" s="24"/>
+      <c r="AZ109" s="24"/>
+      <c r="BA109" s="24"/>
+      <c r="BB109" s="24"/>
+      <c r="BC109" s="24"/>
+      <c r="BD109" s="24"/>
+      <c r="BE109" s="24"/>
+      <c r="BF109" s="24"/>
+      <c r="BG109" s="24"/>
+      <c r="BH109" s="24"/>
+      <c r="BI109" s="24"/>
+      <c r="BJ109" s="24"/>
+      <c r="BK109" s="23"/>
+      <c r="BL109" s="23"/>
+      <c r="BM109" s="23"/>
+      <c r="BN109" s="23"/>
+      <c r="BO109" s="23"/>
+    </row>
+    <row r="110" spans="12:67" x14ac:dyDescent="0.45">
+      <c r="M110" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O110" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH110" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI110" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="AT110" s="2">
+        <v>8</v>
+      </c>
+      <c r="AU110" s="23"/>
+      <c r="AV110" s="2">
+        <v>6</v>
+      </c>
+      <c r="AW110" s="24"/>
+      <c r="AX110" s="24"/>
+      <c r="AY110" s="24"/>
+      <c r="AZ110" s="24"/>
+      <c r="BA110" s="24"/>
+      <c r="BB110" s="24"/>
+      <c r="BC110" s="24"/>
+      <c r="BD110" s="24"/>
+      <c r="BE110" s="24"/>
+      <c r="BF110" s="24"/>
+      <c r="BG110" s="24"/>
+      <c r="BH110" s="24"/>
+      <c r="BI110" s="24"/>
+      <c r="BJ110" s="24"/>
+      <c r="BK110" s="23"/>
+      <c r="BL110" s="23"/>
+      <c r="BM110" s="23"/>
+      <c r="BN110" s="23"/>
+      <c r="BO110" s="23"/>
+    </row>
+    <row r="111" spans="12:67" x14ac:dyDescent="0.45">
+      <c r="AH111" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI111" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT111" s="2">
+        <v>9</v>
+      </c>
+      <c r="AU111" s="23"/>
+      <c r="AV111" s="2">
+        <v>7</v>
+      </c>
+      <c r="AW111" s="24"/>
+      <c r="AX111" s="24"/>
+      <c r="AY111" s="24"/>
+      <c r="AZ111" s="24"/>
+      <c r="BA111" s="24"/>
+      <c r="BB111" s="24"/>
+      <c r="BC111" s="24"/>
+      <c r="BD111" s="24"/>
+      <c r="BE111" s="24"/>
+      <c r="BF111" s="24"/>
+      <c r="BG111" s="24"/>
+      <c r="BH111" s="24"/>
+      <c r="BI111" s="24"/>
+      <c r="BJ111" s="24"/>
+      <c r="BK111" s="23"/>
+      <c r="BL111" s="23"/>
+      <c r="BM111" s="23"/>
+      <c r="BN111" s="23"/>
+      <c r="BO111" s="23"/>
+    </row>
+    <row r="112" spans="12:67" x14ac:dyDescent="0.45">
+      <c r="AH112" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI112" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="AT112" s="2">
+        <v>10</v>
+      </c>
+      <c r="AU112" s="23"/>
+      <c r="AV112" s="2">
+        <v>8</v>
+      </c>
+      <c r="AW112" s="24"/>
+      <c r="AX112" s="24"/>
+      <c r="AY112" s="24"/>
+      <c r="AZ112" s="24"/>
+      <c r="BA112" s="24"/>
+      <c r="BB112" s="24"/>
+      <c r="BC112" s="24"/>
+      <c r="BD112" s="24"/>
+      <c r="BE112" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF112" s="24"/>
+      <c r="BG112" s="24"/>
+      <c r="BH112" s="24"/>
+      <c r="BI112" s="24"/>
+      <c r="BJ112" s="24"/>
+      <c r="BK112" s="23"/>
+      <c r="BL112" s="23"/>
+      <c r="BM112" s="23"/>
+      <c r="BN112" s="23"/>
+      <c r="BO112" s="23"/>
+    </row>
+    <row r="113" spans="13:67" x14ac:dyDescent="0.45">
+      <c r="M113" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O113" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AT113" s="2">
+        <v>11</v>
+      </c>
+      <c r="AU113" s="23"/>
+      <c r="AV113" s="2">
+        <v>9</v>
+      </c>
+      <c r="AW113" s="24"/>
+      <c r="AX113" s="24"/>
+      <c r="AY113" s="24"/>
+      <c r="AZ113" s="24"/>
+      <c r="BA113" s="24"/>
+      <c r="BB113" s="24"/>
+      <c r="BC113" s="24"/>
+      <c r="BD113" s="24"/>
+      <c r="BE113" s="24"/>
+      <c r="BF113" s="24"/>
+      <c r="BG113" s="24"/>
+      <c r="BH113" s="24"/>
+      <c r="BI113" s="24"/>
+      <c r="BJ113" s="24"/>
+      <c r="BK113" s="23"/>
+      <c r="BL113" s="23"/>
+      <c r="BM113" s="23"/>
+      <c r="BN113" s="23"/>
+      <c r="BO113" s="23"/>
+    </row>
+    <row r="114" spans="13:67" x14ac:dyDescent="0.45">
+      <c r="M114" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O114" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT114" s="2">
+        <v>12</v>
+      </c>
+      <c r="AU114" s="23"/>
+      <c r="AV114" s="2">
+        <v>10</v>
+      </c>
+      <c r="AW114" s="24"/>
+      <c r="AX114" s="24"/>
+      <c r="AY114" s="24"/>
+      <c r="AZ114" s="24"/>
+      <c r="BA114" s="24"/>
+      <c r="BB114" s="24"/>
+      <c r="BC114" s="24"/>
+      <c r="BD114" s="24"/>
+      <c r="BE114" s="24"/>
+      <c r="BF114" s="24"/>
+      <c r="BG114" s="24"/>
+      <c r="BH114" s="24"/>
+      <c r="BI114" s="24"/>
+      <c r="BJ114" s="24"/>
+      <c r="BK114" s="23"/>
+      <c r="BL114" s="23"/>
+      <c r="BM114" s="23"/>
+      <c r="BN114" s="23"/>
+      <c r="BO114" s="23"/>
+    </row>
+    <row r="115" spans="13:67" x14ac:dyDescent="0.45">
+      <c r="AT115" s="2">
+        <v>13</v>
+      </c>
+      <c r="AU115" s="23"/>
+      <c r="AV115" s="2">
+        <v>11</v>
+      </c>
+      <c r="AW115" s="24"/>
+      <c r="AX115" s="24"/>
+      <c r="AY115" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="AZ115" s="24"/>
+      <c r="BA115" s="24"/>
+      <c r="BB115" s="24"/>
+      <c r="BC115" s="24"/>
+      <c r="BD115" s="24"/>
+      <c r="BE115" s="24"/>
+      <c r="BF115" s="24"/>
+      <c r="BG115" s="24"/>
+      <c r="BH115" s="24"/>
+      <c r="BI115" s="24"/>
+      <c r="BJ115" s="24"/>
+      <c r="BK115" s="23"/>
+      <c r="BL115" s="23"/>
+      <c r="BM115" s="23"/>
+      <c r="BN115" s="23"/>
+      <c r="BO115" s="23"/>
+    </row>
+    <row r="116" spans="13:67" x14ac:dyDescent="0.45">
+      <c r="M116" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT116" s="2">
+        <v>14</v>
+      </c>
+      <c r="AU116" s="23"/>
+      <c r="AV116" s="2">
+        <v>12</v>
+      </c>
+      <c r="AW116" s="24"/>
+      <c r="AX116" s="24"/>
+      <c r="AY116" s="24"/>
+      <c r="AZ116" s="24"/>
+      <c r="BA116" s="24"/>
+      <c r="BB116" s="24"/>
+      <c r="BC116" s="24"/>
+      <c r="BD116" s="24"/>
+      <c r="BE116" s="24"/>
+      <c r="BF116" s="24"/>
+      <c r="BG116" s="24"/>
+      <c r="BH116" s="24"/>
+      <c r="BI116" s="24"/>
+      <c r="BJ116" s="24"/>
+      <c r="BK116" s="23"/>
+      <c r="BL116" s="23"/>
+      <c r="BM116" s="23"/>
+      <c r="BN116" s="23"/>
+      <c r="BO116" s="23"/>
+    </row>
+    <row r="117" spans="13:67" x14ac:dyDescent="0.45">
+      <c r="AT117" s="2">
+        <v>15</v>
+      </c>
+      <c r="AU117" s="23"/>
+      <c r="AV117" s="2">
+        <v>13</v>
+      </c>
+      <c r="AW117" s="24"/>
+      <c r="AX117" s="24"/>
+      <c r="AY117" s="24"/>
+      <c r="AZ117" s="24"/>
+      <c r="BA117" s="24"/>
+      <c r="BB117" s="24"/>
+      <c r="BC117" s="24"/>
+      <c r="BD117" s="24"/>
+      <c r="BE117" s="24"/>
+      <c r="BF117" s="24"/>
+      <c r="BG117" s="24"/>
+      <c r="BH117" s="24"/>
+      <c r="BI117" s="24"/>
+      <c r="BJ117" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK117" s="23"/>
+      <c r="BL117" s="23"/>
+      <c r="BM117" s="23"/>
+      <c r="BN117" s="23"/>
+      <c r="BO117" s="23"/>
+    </row>
+    <row r="118" spans="13:67" x14ac:dyDescent="0.45">
+      <c r="AT118" s="2">
+        <v>16</v>
+      </c>
+      <c r="AU118" s="23"/>
+      <c r="AV118" s="23"/>
+      <c r="AW118" s="23"/>
+      <c r="AX118" s="23"/>
+      <c r="AY118" s="23"/>
+      <c r="AZ118" s="23"/>
+      <c r="BA118" s="23"/>
+      <c r="BB118" s="23"/>
+      <c r="BC118" s="23"/>
+      <c r="BD118" s="23"/>
+      <c r="BE118" s="23"/>
+      <c r="BF118" s="23"/>
+      <c r="BG118" s="23"/>
+      <c r="BH118" s="23"/>
+      <c r="BI118" s="23"/>
+      <c r="BJ118" s="23"/>
+      <c r="BK118" s="23"/>
+      <c r="BL118" s="23"/>
+      <c r="BM118" s="23"/>
+      <c r="BN118" s="23"/>
+      <c r="BO118" s="23"/>
+    </row>
+    <row r="119" spans="13:67" x14ac:dyDescent="0.45">
+      <c r="AJ119" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="AT119" s="2">
+        <v>17</v>
+      </c>
+      <c r="AU119" s="23"/>
+      <c r="AV119" s="23"/>
+      <c r="AW119" s="23"/>
+      <c r="AX119" s="23"/>
+      <c r="AY119" s="23"/>
+      <c r="AZ119" s="23"/>
+      <c r="BA119" s="23"/>
+      <c r="BB119" s="23"/>
+      <c r="BC119" s="23"/>
+      <c r="BD119" s="23"/>
+      <c r="BE119" s="23"/>
+      <c r="BF119" s="23"/>
+      <c r="BG119" s="23"/>
+      <c r="BH119" s="23"/>
+      <c r="BI119" s="23"/>
+      <c r="BJ119" s="23"/>
+      <c r="BK119" s="23"/>
+      <c r="BL119" s="23"/>
+      <c r="BM119" s="23"/>
+      <c r="BN119" s="23"/>
+      <c r="BO119" s="23"/>
+    </row>
+    <row r="120" spans="13:67" x14ac:dyDescent="0.45">
+      <c r="AJ120" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="AT120" s="2">
+        <v>18</v>
+      </c>
+      <c r="AU120" s="23"/>
+      <c r="AV120" s="23"/>
+      <c r="AW120" s="23"/>
+      <c r="AX120" s="23"/>
+      <c r="AY120" s="23"/>
+      <c r="AZ120" s="23"/>
+      <c r="BA120" s="23"/>
+      <c r="BB120" s="23"/>
+      <c r="BC120" s="23"/>
+      <c r="BD120" s="23"/>
+      <c r="BE120" s="23"/>
+      <c r="BF120" s="23"/>
+      <c r="BG120" s="23"/>
+      <c r="BH120" s="23"/>
+      <c r="BI120" s="23"/>
+      <c r="BJ120" s="23"/>
+      <c r="BK120" s="23"/>
+      <c r="BL120" s="23"/>
+      <c r="BM120" s="23"/>
+      <c r="BN120" s="23"/>
+      <c r="BO120" s="23"/>
+    </row>
+    <row r="121" spans="13:67" x14ac:dyDescent="0.45">
+      <c r="AT121" s="2">
+        <v>19</v>
+      </c>
+      <c r="AU121" s="23"/>
+      <c r="AV121" s="23"/>
+      <c r="AW121" s="23"/>
+      <c r="AX121" s="23"/>
+      <c r="AY121" s="23"/>
+      <c r="AZ121" s="23"/>
+      <c r="BA121" s="23"/>
+      <c r="BB121" s="23"/>
+      <c r="BC121" s="23"/>
+      <c r="BD121" s="23"/>
+      <c r="BE121" s="23"/>
+      <c r="BF121" s="23"/>
+      <c r="BG121" s="23"/>
+      <c r="BH121" s="23"/>
+      <c r="BI121" s="23"/>
+      <c r="BJ121" s="23"/>
+      <c r="BK121" s="23"/>
+      <c r="BL121" s="23"/>
+      <c r="BM121" s="23"/>
+      <c r="BN121" s="23"/>
+      <c r="BO121" s="23"/>
+    </row>
+    <row r="122" spans="13:67" x14ac:dyDescent="0.45">
+      <c r="AT122" s="2">
+        <v>20</v>
+      </c>
+      <c r="AU122" s="23"/>
+      <c r="AV122" s="23"/>
+      <c r="AW122" s="23"/>
+      <c r="AX122" s="23"/>
+      <c r="AY122" s="23"/>
+      <c r="AZ122" s="23"/>
+      <c r="BA122" s="23"/>
+      <c r="BB122" s="23"/>
+      <c r="BC122" s="23"/>
+      <c r="BD122" s="23"/>
+      <c r="BE122" s="23"/>
+      <c r="BF122" s="23"/>
+      <c r="BG122" s="23"/>
+      <c r="BH122" s="23"/>
+      <c r="BI122" s="23"/>
+      <c r="BJ122" s="23"/>
+      <c r="BK122" s="23"/>
+      <c r="BL122" s="23"/>
+      <c r="BM122" s="23"/>
+      <c r="BN122" s="23"/>
+      <c r="BO122" s="23"/>
+    </row>
+    <row r="127" spans="13:67" x14ac:dyDescent="0.45">
+      <c r="AM127" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO127" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="128" spans="13:67" x14ac:dyDescent="0.45">
+      <c r="AM128" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO128" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="129" spans="39:49" x14ac:dyDescent="0.45">
+      <c r="AM129" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO129" s="2">
+        <f>ROUNDDOWN((AO127/2),0)</f>
+        <v>10</v>
+      </c>
+      <c r="AW129" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="130" spans="39:49" x14ac:dyDescent="0.45">
+      <c r="AM130" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO130" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" spans="39:49" x14ac:dyDescent="0.45">
+      <c r="AM131" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO131" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="133" spans="39:49" x14ac:dyDescent="0.45">
+      <c r="AM133" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO133" s="2">
+        <f>AO129 + AO128-AO130</f>
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>